<commit_message>
resolved issue with duct sealing cost calcs
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs.xlsx
+++ b/retrofit_costs/tare_retrofit_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu_tare_model\retrofit_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D8FDF-1E20-456E-A49A-347FEB8DC346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B5208D4-28FB-4F3D-8025-D6575C23EED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="738" activeTab="4" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="738" firstSheet="1" activeTab="4" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="heating_costs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="125">
   <si>
     <t>$/unit</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>retrofit_characteristic</t>
+  </si>
+  <si>
+    <t>10% Leakage</t>
+  </si>
+  <si>
+    <t>20% Leakage</t>
+  </si>
+  <si>
+    <t>30% Leakage</t>
   </si>
 </sst>
 </file>
@@ -3950,17 +3959,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AAB083-F7AB-4F7C-A5E9-54BE3CB88F43}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D24" sqref="D24"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="6" width="15.5546875" customWidth="1"/>
     <col min="7" max="9" width="25.5546875" customWidth="1"/>
     <col min="10" max="10" width="15.5546875" customWidth="1"/>
@@ -4549,8 +4558,8 @@
       <c r="B17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="4">
-        <v>0.1</v>
+      <c r="C17" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D17" t="s">
         <v>93</v>
@@ -4585,8 +4594,8 @@
       <c r="B18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="4">
-        <v>0.2</v>
+      <c r="C18" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="D18" t="s">
         <v>93</v>
@@ -4621,8 +4630,8 @@
       <c r="B19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="4">
-        <v>0.3</v>
+      <c r="C19" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="D19" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
fixed scenario files to conduct stat sampling. need to fix multi-index and visuals in main program
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs.xlsx
+++ b/retrofit_costs/tare_retrofit_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B5208D4-28FB-4F3D-8025-D6575C23EED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D480FBAC-84A3-4684-AC30-41817C2692C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="738" firstSheet="1" activeTab="4" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
@@ -396,9 +396,6 @@
     <t>Rim Joist Insulation: Wall R-10, Exterior</t>
   </si>
   <si>
-    <t xml:space="preserve">Seal Vented Crawlspace: Unvented Crawlspace </t>
-  </si>
-  <si>
     <t>Insulate Finished Attics and Cathedral Ceilings: Finished, R-30</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>30% Leakage</t>
+  </si>
+  <si>
+    <t>Seal Vented Crawlspace: Unvented Crawlspace</t>
   </si>
 </sst>
 </file>
@@ -3959,9 +3959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AAB083-F7AB-4F7C-A5E9-54BE3CB88F43}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3984,10 +3984,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
@@ -4559,7 +4559,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
         <v>93</v>
@@ -4595,7 +4595,7 @@
         <v>111</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
         <v>93</v>
@@ -4631,7 +4631,7 @@
         <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
         <v>93</v>
@@ -4772,7 +4772,7 @@
         <v>109</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>98</v>
@@ -4808,7 +4808,7 @@
         <v>109</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>79</v>

</xml_diff>